<commit_message>
verify Accrual method modified
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3515-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-PERIODIC-OVERDUE-FEE-FLAT-PENALTY-FRE-1-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/3515-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-PERIODIC-OVERDUE-FEE-FLAT-PENALTY-FRE-1-Makerepayment1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="678" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="678" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -145,61 +145,73 @@
     <t>Repayment</t>
   </si>
   <si>
+    <t>Interest Receivable(3)</t>
+  </si>
+  <si>
+    <t>clickonmakerepayment</t>
+  </si>
+  <si>
+    <t>makerepayment</t>
+  </si>
+  <si>
+    <t>repaymenttransactiondate</t>
+  </si>
+  <si>
+    <t>INCOME</t>
+  </si>
+  <si>
+    <t>Income from interest(7)</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>$ 101.92</t>
+  </si>
+  <si>
     <t>L7</t>
   </si>
   <si>
-    <t>$ 10,000</t>
-  </si>
-  <si>
-    <t>Interest Receivable(3)</t>
-  </si>
-  <si>
-    <t>$ 101.92</t>
-  </si>
-  <si>
-    <t>clickonmakerepayment</t>
-  </si>
-  <si>
-    <t>makerepayment</t>
-  </si>
-  <si>
-    <t>repaymenttransactiondate</t>
-  </si>
-  <si>
-    <t>INCOME</t>
-  </si>
-  <si>
-    <t>Income from interest(7)</t>
-  </si>
-  <si>
-    <t>$ 84.82</t>
-  </si>
-  <si>
-    <t>$ 93.91</t>
-  </si>
-  <si>
-    <t>$ 987.72</t>
-  </si>
-  <si>
-    <t>L65</t>
-  </si>
-  <si>
-    <t>L64</t>
-  </si>
-  <si>
-    <t>system</t>
-  </si>
-  <si>
-    <t>L66</t>
-  </si>
-  <si>
-    <t>L67</t>
-  </si>
-  <si>
-    <t>$ 885.8</t>
-  </si>
-  <si>
-    <t>$ 101.92</t>
+    <t>$ 10,000</t>
+  </si>
+  <si>
+    <t>L1564</t>
+  </si>
+  <si>
+    <t>Penalties Receivable(5)</t>
+  </si>
+  <si>
+    <t>$ 100</t>
+  </si>
+  <si>
+    <t>$ 785.8</t>
+  </si>
+  <si>
+    <t>$ 987.72</t>
+  </si>
+  <si>
+    <t>L1561</t>
+  </si>
+  <si>
+    <t>Income from penalties(9)</t>
+  </si>
+  <si>
+    <t>L1565</t>
+  </si>
+  <si>
+    <t>$ 84.82</t>
+  </si>
+  <si>
+    <t>$ 2,900</t>
+  </si>
+  <si>
+    <t>L1566</t>
+  </si>
+  <si>
+    <t>$ 93.91</t>
+  </si>
+  <si>
+    <t>$ 5,400</t>
   </si>
 </sst>
 </file>
@@ -306,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,9 +351,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,15 +690,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="14">
         <v>42036</v>
@@ -1467,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1556,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <v>67</v>
+        <v>1566</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>27</v>
@@ -1531,8 +1567,8 @@
       <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="7">
-        <v>93.91</v>
+      <c r="E2" s="10">
+        <v>5493.91</v>
       </c>
       <c r="F2" s="7">
         <v>0</v>
@@ -1543,8 +1579,8 @@
       <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
-        <v>0</v>
+      <c r="I2" s="9">
+        <v>5400</v>
       </c>
       <c r="J2" s="7">
         <v>0</v>
@@ -1554,7 +1590,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>66</v>
+        <v>1565</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>27</v>
@@ -1565,8 +1601,8 @@
       <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="7">
-        <v>84.82</v>
+      <c r="E3" s="10">
+        <v>2984.82</v>
       </c>
       <c r="F3" s="7">
         <v>0</v>
@@ -1577,8 +1613,8 @@
       <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
-        <v>0</v>
+      <c r="I3" s="9">
+        <v>2900</v>
       </c>
       <c r="J3" s="7">
         <v>0</v>
@@ -1588,7 +1624,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <v>65</v>
+        <v>1564</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>27</v>
@@ -1603,7 +1639,7 @@
         <v>987.72</v>
       </c>
       <c r="F4" s="7">
-        <v>885.8</v>
+        <v>785.8</v>
       </c>
       <c r="G4" s="7">
         <v>101.92</v>
@@ -1612,17 +1648,17 @@
         <v>0</v>
       </c>
       <c r="I4" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="10">
-        <v>9114.2000000000007</v>
+        <v>9214.2000000000007</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>62</v>
+        <v>1561</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>27</v>
@@ -1656,7 +1692,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>59</v>
+        <v>1560</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>27</v>
@@ -1695,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1742,7 @@
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1735,7 +1771,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>13</v>
       </c>
@@ -1746,7 +1782,7 @@
         <v>42005</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>36</v>
@@ -1758,12 +1794,11 @@
         <v>38</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>14</v>
       </c>
@@ -1774,7 +1809,7 @@
         <v>42005</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>36</v>
@@ -1787,21 +1822,21 @@
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="12"/>
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,85 +1881,112 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>93</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="18">
+        <v>2582</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="19">
         <v>42036</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2583</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="19">
+        <v>42036</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>2584</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="19">
+        <v>42036</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>94</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="H4" s="17"/>
+      <c r="I4" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>2585</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C5" s="19">
         <v>42036</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>95</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="13">
-        <v>42036</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="G5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="12"/>
+      <c r="H5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1933,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:I15"/>
+      <selection activeCell="A12" sqref="A12:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,211 +2042,327 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>85</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="20">
+        <v>2562</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="21">
+        <v>42036</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>2563</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="21">
+        <v>42036</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>2564</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="21">
+        <v>42036</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>2565</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="21">
+        <v>42036</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>2586</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="23">
+        <v>42064</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>2587</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="23">
+        <v>42064</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>2588</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="23">
+        <v>42064</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>2589</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="23">
+        <v>42064</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>2590</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="25">
         <v>42095</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D12" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>86</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="F12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>2591</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C13" s="25">
         <v>42095</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>91</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="D13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>2592</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C14" s="25">
         <v>42095</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="D14" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>92</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="G14" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>2593</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C15" s="25">
         <v>42095</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D15" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>96</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="13">
-        <v>42064</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>97</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="13">
-        <v>42064</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>98</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="13">
-        <v>42095</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="G15" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>99</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="13">
-        <v>42095</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>51</v>
+      <c r="H15" s="26"/>
+      <c r="I15" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>